<commit_message>
added data for SCI
</commit_message>
<xml_diff>
--- a/data/GSCI/2017.xlsx
+++ b/data/GSCI/2017.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4B3614-6904-4F3F-A64C-2949BAFF89B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{0E4B3614-6904-4F3F-A64C-2949BAFF89B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE4FCC33-DAE3-48A6-9B8F-D5C872286A67}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Data usage" sheetId="2" r:id="rId2"/>
+    <sheet name="sci" sheetId="3" r:id="rId2"/>
+    <sheet name="Data usage" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Data!$B$4:$L$184</definedName>
@@ -22,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="204">
   <si>
     <t>Country</t>
   </si>
@@ -636,6 +642,12 @@
   </si>
   <si>
     <t>The Global Sustainability Competitiveness Index 2017</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>sci</t>
   </si>
 </sst>
 </file>
@@ -954,19 +966,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -980,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -993,13 +1005,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1508,24 +1520,24 @@
   <dimension ref="B1:P188"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="R1" sqref="R1:S1048576"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5:B184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="26" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="9" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="9" customWidth="1"/>
+    <col min="5" max="14" width="11.5546875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="36" t="s">
         <v>201</v>
       </c>
@@ -1543,7 +1555,7 @@
       <c r="N2" s="35"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="37" t="s">
         <v>0</v>
       </c>
@@ -1572,7 +1584,7 @@
       </c>
       <c r="N3" s="39"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
         <v>1</v>
@@ -1611,7 +1623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
@@ -1652,7 +1664,7 @@
         <v>55.07112894400877</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1705,7 @@
         <v>58.629399963523625</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1734,7 +1746,7 @@
         <v>58.083895677548803</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1775,7 +1787,7 @@
         <v>57.089184752872534</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1816,7 +1828,7 @@
         <v>55.021885828925768</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1857,7 +1869,7 @@
         <v>49.93944920663872</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1898,7 +1910,7 @@
         <v>56.432609885099396</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1939,7 +1951,7 @@
         <v>54.907897136604063</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +1992,7 @@
         <v>46.011307678278321</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2021,7 +2033,7 @@
         <v>47.628123290169633</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2062,7 +2074,7 @@
         <v>55.950209739193888</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2103,7 +2115,7 @@
         <v>58.447677436552148</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -2144,7 +2156,7 @@
         <v>47.564107240561739</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
@@ -2185,7 +2197,7 @@
         <v>56.583804486594936</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
@@ -2226,7 +2238,7 @@
         <v>46.697063651285802</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>45</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>56.303665876345072</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
@@ -2308,7 +2320,7 @@
         <v>52.61626345567619</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>50.873426956045975</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2390,7 +2402,7 @@
         <v>52.968265548057644</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2431,7 +2443,7 @@
         <v>56.361480941090647</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>50.249863213569228</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>53</v>
       </c>
@@ -2513,7 +2525,7 @@
         <v>49.769286886740858</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2554,7 +2566,7 @@
         <v>44.186576691592201</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
@@ -2595,7 +2607,7 @@
         <v>49.384461061462716</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
@@ -2636,7 +2648,7 @@
         <v>47.893488965894591</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>42</v>
       </c>
@@ -2677,7 +2689,7 @@
         <v>54.043224512128418</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>54</v>
       </c>
@@ -2718,7 +2730,7 @@
         <v>45.514316979755606</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2759,7 +2771,7 @@
         <v>55.527995622834226</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="2" t="s">
         <v>46</v>
       </c>
@@ -2800,7 +2812,7 @@
         <v>36.408900237096482</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>43</v>
       </c>
@@ -2841,7 +2853,7 @@
         <v>40.642531460879091</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
@@ -2882,7 +2894,7 @@
         <v>49.888747036294014</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>30</v>
       </c>
@@ -2923,7 +2935,7 @@
         <v>48.345978478934889</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>44</v>
       </c>
@@ -2964,7 +2976,7 @@
         <v>51.085172350902788</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="2" t="s">
         <v>32</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>46.16396133503558</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="2" t="s">
         <v>59</v>
       </c>
@@ -3046,7 +3058,7 @@
         <v>36.949297829655301</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
@@ -3087,7 +3099,7 @@
         <v>49.089002370964792</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="2" t="s">
         <v>37</v>
       </c>
@@ -3128,7 +3140,7 @@
         <v>49.6771840233449</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="2" t="s">
         <v>49</v>
       </c>
@@ -3169,7 +3181,7 @@
         <v>48.385920116724435</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="2" t="s">
         <v>35</v>
       </c>
@@ -3210,7 +3222,7 @@
         <v>41.680466897683758</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>52</v>
       </c>
@@ -3251,7 +3263,7 @@
         <v>42.544227612620837</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>61</v>
       </c>
@@ -3292,7 +3304,7 @@
         <v>46.163049425497</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>29</v>
       </c>
@@ -3333,7 +3345,7 @@
         <v>37.881451759985417</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>38</v>
       </c>
@@ -3374,7 +3386,7 @@
         <v>36.583986868502642</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>67</v>
       </c>
@@ -3415,7 +3427,7 @@
         <v>45.453583804486613</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B49" s="2" t="s">
         <v>100</v>
       </c>
@@ -3456,7 +3468,7 @@
         <v>48.409082619004209</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>62</v>
       </c>
@@ -3497,7 +3509,7 @@
         <v>41.086084260441361</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>28</v>
       </c>
@@ -3538,7 +3550,7 @@
         <v>39.43735181469998</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>76</v>
       </c>
@@ -3579,7 +3591,7 @@
         <v>44.911544774758354</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
         <v>89</v>
       </c>
@@ -3620,7 +3632,7 @@
         <v>48.739193871967885</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
         <v>74</v>
       </c>
@@ -3661,7 +3673,7 @@
         <v>48.407805945650189</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B55" s="2" t="s">
         <v>56</v>
       </c>
@@ -3702,7 +3714,7 @@
         <v>44.148823636695241</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B56" s="2" t="s">
         <v>50</v>
       </c>
@@ -3743,7 +3755,7 @@
         <v>32.446470910085722</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>112</v>
       </c>
@@ -3784,7 +3796,7 @@
         <v>46.24439175633777</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B58" s="2" t="s">
         <v>39</v>
       </c>
@@ -3825,7 +3837,7 @@
         <v>53.657122013496256</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
         <v>57</v>
       </c>
@@ -3866,7 +3878,7 @@
         <v>38.951851176363306</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
         <v>107</v>
       </c>
@@ -3907,7 +3919,7 @@
         <v>48.992453948568318</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
         <v>60</v>
       </c>
@@ -3948,7 +3960,7 @@
         <v>32.432609885099403</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
         <v>68</v>
       </c>
@@ -3989,7 +4001,7 @@
         <v>46.01842057267919</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
         <v>70</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>50.669888747036296</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
         <v>47</v>
       </c>
@@ -4071,7 +4083,7 @@
         <v>39.473463432427501</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
         <v>51</v>
       </c>
@@ -4112,7 +4124,7 @@
         <v>41.497902608061281</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
         <v>73</v>
       </c>
@@ -4153,7 +4165,7 @@
         <v>46.286521977019895</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
         <v>102</v>
       </c>
@@ -4194,7 +4206,7 @@
         <v>37.643443370417664</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
         <v>86</v>
       </c>
@@ -4235,7 +4247,7 @@
         <v>40.202079153747952</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
         <v>80</v>
       </c>
@@ -4276,7 +4288,7 @@
         <v>34.90534378989603</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
         <v>48</v>
       </c>
@@ -4317,7 +4329,7 @@
         <v>42.702899872332658</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
         <v>90</v>
       </c>
@@ -4358,7 +4370,7 @@
         <v>40.310596388838235</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
         <v>75</v>
       </c>
@@ -4399,7 +4411,7 @@
         <v>37.890023709648013</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
         <v>63</v>
       </c>
@@ -4440,7 +4452,7 @@
         <v>38.628123290169626</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>101</v>
       </c>
@@ -4481,7 +4493,7 @@
         <v>39.804668976837497</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
         <v>98</v>
       </c>
@@ -4522,7 +4534,7 @@
         <v>46.538313227899224</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
         <v>65</v>
       </c>
@@ -4563,7 +4575,7 @@
         <v>35.623381360569041</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
         <v>124</v>
       </c>
@@ -4604,7 +4616,7 @@
         <v>45.498449753784421</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
         <v>127</v>
       </c>
@@ -4645,7 +4657,7 @@
         <v>49.827284333394132</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
         <v>96</v>
       </c>
@@ -4686,7 +4698,7 @@
         <v>43.127484953492619</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
         <v>55</v>
       </c>
@@ -4727,7 +4739,7 @@
         <v>46.597300747765836</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
         <v>114</v>
       </c>
@@ -4768,7 +4780,7 @@
         <v>33.095568119642536</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
         <v>34</v>
       </c>
@@ -4809,7 +4821,7 @@
         <v>41.474010578150633</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
         <v>83</v>
       </c>
@@ -4850,7 +4862,7 @@
         <v>45.357286157213203</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>134</v>
       </c>
@@ -4891,7 +4903,7 @@
         <v>36.185300018238188</v>
       </c>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>94</v>
       </c>
@@ -4932,7 +4944,7 @@
         <v>32.31825642896225</v>
       </c>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B86" s="2" t="s">
         <v>99</v>
       </c>
@@ -4973,7 +4985,7 @@
         <v>38.484041583074955</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
         <v>58</v>
       </c>
@@ -5014,7 +5026,7 @@
         <v>42.748130585445928</v>
       </c>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
         <v>69</v>
       </c>
@@ -5055,7 +5067,7 @@
         <v>45.623928506292195</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
         <v>71</v>
       </c>
@@ -5096,7 +5108,7 @@
         <v>45.113259164690852</v>
       </c>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>87</v>
       </c>
@@ -5137,7 +5149,7 @@
         <v>38.146817435710375</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>93</v>
       </c>
@@ -5178,7 +5190,7 @@
         <v>34.727521429874159</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>85</v>
       </c>
@@ -5219,7 +5231,7 @@
         <v>34.134050702170349</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B93" s="2" t="s">
         <v>77</v>
       </c>
@@ -5260,7 +5272,7 @@
         <v>33.570490607331756</v>
       </c>
     </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
         <v>66</v>
       </c>
@@ -5301,7 +5313,7 @@
         <v>44.538573773481687</v>
       </c>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B95" s="2" t="s">
         <v>91</v>
       </c>
@@ -5342,7 +5354,7 @@
         <v>45.322998358562828</v>
       </c>
     </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B96" s="2" t="s">
         <v>97</v>
       </c>
@@ -5383,7 +5395,7 @@
         <v>38.267189494802125</v>
       </c>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B97" s="2" t="s">
         <v>78</v>
       </c>
@@ -5424,7 +5436,7 @@
         <v>30.15739558635784</v>
       </c>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B98" s="2" t="s">
         <v>82</v>
       </c>
@@ -5465,7 +5477,7 @@
         <v>37.83643658912672</v>
       </c>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B99" s="2" t="s">
         <v>95</v>
       </c>
@@ -5506,7 +5518,7 @@
         <v>52.062009848623028</v>
       </c>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B100" s="2" t="s">
         <v>64</v>
       </c>
@@ -5547,7 +5559,7 @@
         <v>52.760714937078248</v>
       </c>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B101" s="2" t="s">
         <v>81</v>
       </c>
@@ -5588,7 +5600,7 @@
         <v>50.154659857742111</v>
       </c>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
         <v>105</v>
       </c>
@@ -5629,7 +5641,7 @@
         <v>39.826007660040119</v>
       </c>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">
         <v>92</v>
       </c>
@@ -5670,7 +5682,7 @@
         <v>41.190224329746485</v>
       </c>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B104" s="2" t="s">
         <v>41</v>
       </c>
@@ -5711,7 +5723,7 @@
         <v>44.304760167791351</v>
       </c>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
         <v>103</v>
       </c>
@@ -5752,7 +5764,7 @@
         <v>29.326281232901692</v>
       </c>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
         <v>142</v>
       </c>
@@ -5793,7 +5805,7 @@
         <v>32.522888929418208</v>
       </c>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B107" s="2" t="s">
         <v>117</v>
       </c>
@@ -5834,7 +5846,7 @@
         <v>39.777858836403439</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B108" s="2" t="s">
         <v>118</v>
       </c>
@@ -5875,7 +5887,7 @@
         <v>37.970818894765642</v>
       </c>
     </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B109" s="2" t="s">
         <v>120</v>
       </c>
@@ -5916,7 +5928,7 @@
         <v>41.607149370782416</v>
       </c>
     </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B110" s="2" t="s">
         <v>72</v>
       </c>
@@ -5957,7 +5969,7 @@
         <v>42.822360021885842</v>
       </c>
     </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B111" s="2" t="s">
         <v>125</v>
       </c>
@@ -5998,7 +6010,7 @@
         <v>40.231625022797743</v>
       </c>
     </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B112" s="2" t="s">
         <v>146</v>
       </c>
@@ -6039,7 +6051,7 @@
         <v>35.116724420937445</v>
       </c>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B113" s="2" t="s">
         <v>109</v>
       </c>
@@ -6080,7 +6092,7 @@
         <v>34.453036658763452</v>
       </c>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B114" s="2" t="s">
         <v>113</v>
       </c>
@@ -6121,7 +6133,7 @@
         <v>46.192777676454497</v>
       </c>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
         <v>148</v>
       </c>
@@ -6162,7 +6174,7 @@
         <v>41.113988692321726</v>
       </c>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
         <v>110</v>
       </c>
@@ -6203,7 +6215,7 @@
         <v>36.666058726974285</v>
       </c>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
         <v>106</v>
       </c>
@@ -6244,7 +6256,7 @@
         <v>39.461895208566737</v>
       </c>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B118" s="2" t="s">
         <v>121</v>
       </c>
@@ -6285,7 +6297,7 @@
         <v>37.303483494437351</v>
       </c>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B119" s="2" t="s">
         <v>79</v>
       </c>
@@ -6326,7 +6338,7 @@
         <v>42.058726974284149</v>
       </c>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B120" s="2" t="s">
         <v>163</v>
       </c>
@@ -6367,7 +6379,7 @@
         <v>36.641437169432798</v>
       </c>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B121" s="2" t="s">
         <v>164</v>
       </c>
@@ -6408,7 +6420,7 @@
         <v>32.771840233448842</v>
       </c>
     </row>
-    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B122" s="2" t="s">
         <v>160</v>
       </c>
@@ -6449,7 +6461,7 @@
         <v>39.839139157395579</v>
       </c>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B123" s="2" t="s">
         <v>131</v>
       </c>
@@ -6490,7 +6502,7 @@
         <v>36.859018785336502</v>
       </c>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B124" s="2" t="s">
         <v>119</v>
       </c>
@@ -6531,7 +6543,7 @@
         <v>36.299288710559914</v>
       </c>
     </row>
-    <row r="125" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B125" s="2" t="s">
         <v>136</v>
       </c>
@@ -6572,7 +6584,7 @@
         <v>41.103045777858839</v>
       </c>
     </row>
-    <row r="126" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B126" s="2" t="s">
         <v>147</v>
       </c>
@@ -6613,7 +6625,7 @@
         <v>35.203355827101952</v>
       </c>
     </row>
-    <row r="127" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B127" s="2" t="s">
         <v>111</v>
       </c>
@@ -6654,7 +6666,7 @@
         <v>33.467444829472917</v>
       </c>
     </row>
-    <row r="128" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B128" s="2" t="s">
         <v>104</v>
       </c>
@@ -6695,7 +6707,7 @@
         <v>38.109976290351995</v>
       </c>
     </row>
-    <row r="129" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B129" s="2" t="s">
         <v>144</v>
       </c>
@@ -6736,7 +6748,7 @@
         <v>44.201167244209373</v>
       </c>
     </row>
-    <row r="130" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B130" s="2" t="s">
         <v>123</v>
       </c>
@@ -6777,7 +6789,7 @@
         <v>43.396498267371875</v>
       </c>
     </row>
-    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B131" s="2" t="s">
         <v>149</v>
       </c>
@@ -6818,7 +6830,7 @@
         <v>37.875433157030827</v>
       </c>
     </row>
-    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B132" s="2" t="s">
         <v>193</v>
       </c>
@@ -6859,7 +6871,7 @@
         <v>38.936713478022988</v>
       </c>
     </row>
-    <row r="133" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B133" s="2" t="s">
         <v>84</v>
       </c>
@@ -6900,7 +6912,7 @@
         <v>32.392121101586724</v>
       </c>
     </row>
-    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B134" s="2" t="s">
         <v>130</v>
       </c>
@@ -6941,7 +6953,7 @@
         <v>30.914098121466349</v>
       </c>
     </row>
-    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B135" s="2" t="s">
         <v>128</v>
       </c>
@@ -6982,7 +6994,7 @@
         <v>32.285245303665874</v>
       </c>
     </row>
-    <row r="136" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B136" s="2" t="s">
         <v>192</v>
       </c>
@@ -7023,7 +7035,7 @@
         <v>37.016596753602052</v>
       </c>
     </row>
-    <row r="137" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B137" s="2" t="s">
         <v>177</v>
       </c>
@@ -7064,7 +7076,7 @@
         <v>35.668429691774577</v>
       </c>
     </row>
-    <row r="138" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B138" s="2" t="s">
         <v>165</v>
       </c>
@@ -7105,7 +7117,7 @@
         <v>38.668794455590003</v>
       </c>
     </row>
-    <row r="139" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B139" s="2" t="s">
         <v>135</v>
       </c>
@@ -7146,7 +7158,7 @@
         <v>36.580521612256071</v>
       </c>
     </row>
-    <row r="140" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B140" s="2" t="s">
         <v>126</v>
       </c>
@@ -7187,7 +7199,7 @@
         <v>29.535473281050521</v>
       </c>
     </row>
-    <row r="141" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B141" s="2" t="s">
         <v>168</v>
       </c>
@@ -7228,7 +7240,7 @@
         <v>40.964800291811052</v>
       </c>
     </row>
-    <row r="142" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B142" s="2" t="s">
         <v>150</v>
       </c>
@@ -7269,7 +7281,7 @@
         <v>35.967536020426778</v>
       </c>
     </row>
-    <row r="143" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B143" s="2" t="s">
         <v>143</v>
       </c>
@@ -7310,7 +7322,7 @@
         <v>43.146999817618088</v>
       </c>
     </row>
-    <row r="144" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B144" s="2" t="s">
         <v>141</v>
       </c>
@@ -7351,7 +7363,7 @@
         <v>35.66842969177457</v>
       </c>
     </row>
-    <row r="145" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B145" s="2" t="s">
         <v>129</v>
       </c>
@@ -7392,7 +7404,7 @@
         <v>36.25606419843151</v>
       </c>
     </row>
-    <row r="146" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B146" s="2" t="s">
         <v>153</v>
       </c>
@@ -7433,7 +7445,7 @@
         <v>38.391756337771298</v>
       </c>
     </row>
-    <row r="147" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B147" s="2" t="s">
         <v>198</v>
       </c>
@@ -7474,7 +7486,7 @@
         <v>39.179463797191325</v>
       </c>
     </row>
-    <row r="148" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B148" s="2" t="s">
         <v>116</v>
       </c>
@@ -7515,7 +7527,7 @@
         <v>33.46270289987234</v>
       </c>
     </row>
-    <row r="149" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B149" s="2" t="s">
         <v>133</v>
       </c>
@@ -7556,7 +7568,7 @@
         <v>42.605690315520711</v>
       </c>
     </row>
-    <row r="150" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B150" s="2" t="s">
         <v>155</v>
       </c>
@@ -7597,7 +7609,7 @@
         <v>32.084442823271928</v>
       </c>
     </row>
-    <row r="151" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B151" s="2" t="s">
         <v>132</v>
       </c>
@@ -7638,7 +7650,7 @@
         <v>31.83695057450301</v>
       </c>
     </row>
-    <row r="152" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B152" s="2" t="s">
         <v>194</v>
       </c>
@@ -7679,7 +7691,7 @@
         <v>39.589959875980298</v>
       </c>
     </row>
-    <row r="153" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B153" s="2" t="s">
         <v>158</v>
       </c>
@@ -7720,7 +7732,7 @@
         <v>41.790990333758891</v>
       </c>
     </row>
-    <row r="154" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B154" s="2" t="s">
         <v>154</v>
       </c>
@@ -7761,7 +7773,7 @@
         <v>42.885828925770561</v>
       </c>
     </row>
-    <row r="155" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B155" s="2" t="s">
         <v>156</v>
       </c>
@@ -7802,7 +7814,7 @@
         <v>35.613167973737006</v>
       </c>
     </row>
-    <row r="156" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B156" s="2" t="s">
         <v>122</v>
       </c>
@@ -7843,7 +7855,7 @@
         <v>33.107058179828556</v>
       </c>
     </row>
-    <row r="157" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B157" s="2" t="s">
         <v>139</v>
       </c>
@@ -7884,7 +7896,7 @@
         <v>41.301842057267919</v>
       </c>
     </row>
-    <row r="158" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B158" s="2" t="s">
         <v>151</v>
       </c>
@@ -7925,7 +7937,7 @@
         <v>39.265912821448111</v>
       </c>
     </row>
-    <row r="159" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B159" s="2" t="s">
         <v>167</v>
       </c>
@@ -7966,7 +7978,7 @@
         <v>32.328469815794271</v>
       </c>
     </row>
-    <row r="160" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B160" s="2" t="s">
         <v>140</v>
       </c>
@@ -8007,7 +8019,7 @@
         <v>37.659675360204268</v>
       </c>
     </row>
-    <row r="161" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B161" s="2" t="s">
         <v>108</v>
       </c>
@@ -8048,7 +8060,7 @@
         <v>44.667335400328305</v>
       </c>
     </row>
-    <row r="162" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B162" s="2" t="s">
         <v>145</v>
       </c>
@@ -8089,7 +8101,7 @@
         <v>31.963341236549336</v>
       </c>
     </row>
-    <row r="163" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B163" s="2" t="s">
         <v>157</v>
       </c>
@@ -8130,7 +8142,7 @@
         <v>30.708371329564109</v>
       </c>
     </row>
-    <row r="164" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B164" s="2" t="s">
         <v>138</v>
       </c>
@@ -8171,7 +8183,7 @@
         <v>33.616268466168151</v>
       </c>
     </row>
-    <row r="165" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B165" s="2" t="s">
         <v>170</v>
       </c>
@@ -8212,7 +8224,7 @@
         <v>34.391026810140438</v>
       </c>
     </row>
-    <row r="166" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B166" s="2" t="s">
         <v>169</v>
       </c>
@@ -8253,7 +8265,7 @@
         <v>32.971366040488796</v>
       </c>
     </row>
-    <row r="167" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B167" s="2" t="s">
         <v>162</v>
       </c>
@@ -8294,7 +8306,7 @@
         <v>28.657851541127116</v>
       </c>
     </row>
-    <row r="168" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B168" s="2" t="s">
         <v>152</v>
       </c>
@@ -8335,7 +8347,7 @@
         <v>29.531096115265367</v>
       </c>
     </row>
-    <row r="169" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B169" s="2" t="s">
         <v>115</v>
       </c>
@@ -8376,7 +8388,7 @@
         <v>46.031369688126937</v>
       </c>
     </row>
-    <row r="170" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B170" s="2" t="s">
         <v>174</v>
       </c>
@@ -8417,7 +8429,7 @@
         <v>38.752507751231072</v>
       </c>
     </row>
-    <row r="171" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B171" s="2" t="s">
         <v>166</v>
       </c>
@@ -8458,7 +8470,7 @@
         <v>38.857377348167063</v>
       </c>
     </row>
-    <row r="172" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B172" s="2" t="s">
         <v>178</v>
       </c>
@@ -8499,7 +8511,7 @@
         <v>36.863395951121653</v>
       </c>
     </row>
-    <row r="173" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B173" s="2" t="s">
         <v>137</v>
       </c>
@@ -8540,7 +8552,7 @@
         <v>32.577603501732632</v>
       </c>
     </row>
-    <row r="174" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B174" s="2" t="s">
         <v>161</v>
       </c>
@@ -8581,7 +8593,7 @@
         <v>34.042631770928324</v>
       </c>
     </row>
-    <row r="175" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B175" s="2" t="s">
         <v>159</v>
       </c>
@@ -8622,7 +8634,7 @@
         <v>34.198978661316808</v>
       </c>
     </row>
-    <row r="176" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B176" s="2" t="s">
         <v>171</v>
       </c>
@@ -8663,7 +8675,7 @@
         <v>38.435345613715121</v>
       </c>
     </row>
-    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B177" s="2" t="s">
         <v>175</v>
       </c>
@@ -8704,7 +8716,7 @@
         <v>36.130585445923771</v>
       </c>
     </row>
-    <row r="178" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B178" s="2" t="s">
         <v>172</v>
       </c>
@@ -8745,7 +8757,7 @@
         <v>35.23227638675386</v>
       </c>
     </row>
-    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B179" s="2" t="s">
         <v>199</v>
       </c>
@@ -8786,7 +8798,7 @@
         <v>29.490789713660408</v>
       </c>
     </row>
-    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B180" s="2" t="s">
         <v>173</v>
       </c>
@@ -8827,7 +8839,7 @@
         <v>30.998358562830568</v>
       </c>
     </row>
-    <row r="181" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B181" s="2" t="s">
         <v>200</v>
       </c>
@@ -8868,7 +8880,7 @@
         <v>35.093118991167508</v>
       </c>
     </row>
-    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B182" s="2" t="s">
         <v>88</v>
       </c>
@@ -8909,7 +8921,7 @@
         <v>32.98084989968995</v>
       </c>
     </row>
-    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B183" s="2" t="s">
         <v>179</v>
       </c>
@@ -8950,7 +8962,7 @@
         <v>30.920116724420943</v>
       </c>
     </row>
-    <row r="184" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B184" s="2" t="s">
         <v>176</v>
       </c>
@@ -8991,7 +9003,7 @@
         <v>33.623381360569034</v>
       </c>
     </row>
-    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B185" s="10"/>
       <c r="C185" s="11"/>
       <c r="D185" s="12"/>
@@ -9006,7 +9018,7 @@
       <c r="M185" s="13"/>
       <c r="N185" s="14"/>
     </row>
-    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B186" s="15" t="s">
         <v>181</v>
       </c>
@@ -9041,7 +9053,7 @@
         <v>41.407988510390268</v>
       </c>
     </row>
-    <row r="187" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B187" s="15" t="s">
         <v>182</v>
       </c>
@@ -9076,7 +9088,7 @@
         <v>58.629399963523625</v>
       </c>
     </row>
-    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B188" s="15" t="s">
         <v>183</v>
       </c>
@@ -9113,7 +9125,7 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:L184" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="B5:N184">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:N184">
       <sortCondition ref="C4:C184"/>
     </sortState>
   </autoFilter>
@@ -9124,22 +9136,1485 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3234260-63CD-4130-8A0A-6E0EAD49CCEB}">
+  <dimension ref="A1:B181"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="53">
+        <v>55.07112894400877</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="53">
+        <v>58.629399963523625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="53">
+        <v>58.083895677548803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="53">
+        <v>57.089184752872534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="53">
+        <v>55.021885828925768</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="53">
+        <v>49.93944920663872</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="53">
+        <v>56.432609885099396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="53">
+        <v>54.907897136604063</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="53">
+        <v>46.011307678278321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="53">
+        <v>47.628123290169633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="53">
+        <v>55.950209739193888</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="53">
+        <v>58.447677436552148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="53">
+        <v>47.564107240561739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="53">
+        <v>56.583804486594936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="53">
+        <v>46.697063651285802</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="53">
+        <v>56.303665876345072</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="53">
+        <v>52.61626345567619</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="53">
+        <v>50.873426956045975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="53">
+        <v>52.968265548057644</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="53">
+        <v>56.361480941090647</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="53">
+        <v>50.249863213569228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="53">
+        <v>49.769286886740858</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="53">
+        <v>44.186576691592201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="53">
+        <v>49.384461061462716</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="53">
+        <v>47.893488965894591</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="53">
+        <v>54.043224512128418</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="53">
+        <v>45.514316979755606</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="53">
+        <v>55.527995622834226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="53">
+        <v>36.408900237096482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="53">
+        <v>40.642531460879091</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="53">
+        <v>49.888747036294014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="53">
+        <v>48.345978478934889</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="53">
+        <v>51.085172350902788</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="53">
+        <v>46.16396133503558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="53">
+        <v>36.949297829655301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="53">
+        <v>49.089002370964792</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="53">
+        <v>49.6771840233449</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="53">
+        <v>48.385920116724435</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="53">
+        <v>41.680466897683758</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="53">
+        <v>42.544227612620837</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="53">
+        <v>46.163049425497</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="53">
+        <v>37.881451759985417</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="53">
+        <v>36.583986868502642</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="53">
+        <v>45.453583804486613</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="53">
+        <v>48.409082619004209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="53">
+        <v>41.086084260441361</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="53">
+        <v>39.43735181469998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="53">
+        <v>44.911544774758354</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="53">
+        <v>48.739193871967885</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="53">
+        <v>48.407805945650189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="53">
+        <v>44.148823636695241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="53">
+        <v>32.446470910085722</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="53">
+        <v>46.24439175633777</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B55" s="53">
+        <v>53.657122013496256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="53">
+        <v>38.951851176363306</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B57" s="53">
+        <v>48.992453948568318</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="53">
+        <v>32.432609885099403</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="53">
+        <v>46.01842057267919</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" s="53">
+        <v>50.669888747036296</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="53">
+        <v>39.473463432427501</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B62" s="53">
+        <v>41.497902608061281</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" s="53">
+        <v>46.286521977019895</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="53">
+        <v>37.643443370417664</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" s="53">
+        <v>40.202079153747952</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66" s="53">
+        <v>34.90534378989603</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="53">
+        <v>42.702899872332658</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68" s="53">
+        <v>40.310596388838235</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" s="53">
+        <v>37.890023709648013</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" s="53">
+        <v>38.628123290169626</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" s="53">
+        <v>39.804668976837497</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" s="53">
+        <v>46.538313227899224</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="53">
+        <v>35.623381360569041</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" s="53">
+        <v>45.498449753784421</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B75" s="53">
+        <v>49.827284333394132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="53">
+        <v>43.127484953492619</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77" s="53">
+        <v>46.597300747765836</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" s="53">
+        <v>33.095568119642536</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="53">
+        <v>41.474010578150633</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="53">
+        <v>45.357286157213203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" s="53">
+        <v>36.185300018238188</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="53">
+        <v>32.31825642896225</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" s="53">
+        <v>38.484041583074955</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B84" s="53">
+        <v>42.748130585445928</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="53">
+        <v>45.623928506292195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B86" s="53">
+        <v>45.113259164690852</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" s="53">
+        <v>38.146817435710375</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" s="53">
+        <v>34.727521429874159</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="53">
+        <v>34.134050702170349</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B90" s="53">
+        <v>33.570490607331756</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B91" s="53">
+        <v>44.538573773481687</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" s="53">
+        <v>45.322998358562828</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="53">
+        <v>38.267189494802125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B94" s="53">
+        <v>30.15739558635784</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B95" s="53">
+        <v>37.83643658912672</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" s="53">
+        <v>52.062009848623028</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B97" s="53">
+        <v>52.760714937078248</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" s="53">
+        <v>50.154659857742111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99" s="53">
+        <v>39.826007660040119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B100" s="53">
+        <v>41.190224329746485</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B101" s="53">
+        <v>44.304760167791351</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B102" s="53">
+        <v>29.326281232901692</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B103" s="53">
+        <v>32.522888929418208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104" s="53">
+        <v>39.777858836403439</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B105" s="53">
+        <v>37.970818894765642</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B106" s="53">
+        <v>41.607149370782416</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B107" s="53">
+        <v>42.822360021885842</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B108" s="53">
+        <v>40.231625022797743</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B109" s="53">
+        <v>35.116724420937445</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" s="53">
+        <v>34.453036658763452</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B111" s="53">
+        <v>46.192777676454497</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B112" s="53">
+        <v>41.113988692321726</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B113" s="53">
+        <v>36.666058726974285</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B114" s="53">
+        <v>39.461895208566737</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B115" s="53">
+        <v>37.303483494437351</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B116" s="53">
+        <v>42.058726974284149</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B117" s="53">
+        <v>36.641437169432798</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B118" s="53">
+        <v>32.771840233448842</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B119" s="53">
+        <v>39.839139157395579</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B120" s="53">
+        <v>36.859018785336502</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B121" s="53">
+        <v>36.299288710559914</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B122" s="53">
+        <v>41.103045777858839</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B123" s="53">
+        <v>35.203355827101952</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B124" s="53">
+        <v>33.467444829472917</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B125" s="53">
+        <v>38.109976290351995</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B126" s="53">
+        <v>44.201167244209373</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B127" s="53">
+        <v>43.396498267371875</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B128" s="53">
+        <v>37.875433157030827</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B129" s="53">
+        <v>38.936713478022988</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B130" s="53">
+        <v>32.392121101586724</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131" s="53">
+        <v>30.914098121466349</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B132" s="53">
+        <v>32.285245303665874</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B133" s="53">
+        <v>37.016596753602052</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B134" s="53">
+        <v>35.668429691774577</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B135" s="53">
+        <v>38.668794455590003</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B136" s="53">
+        <v>36.580521612256071</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B137" s="53">
+        <v>29.535473281050521</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B138" s="53">
+        <v>40.964800291811052</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B139" s="53">
+        <v>35.967536020426778</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B140" s="53">
+        <v>43.146999817618088</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="53">
+        <v>35.66842969177457</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B142" s="53">
+        <v>36.25606419843151</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B143" s="53">
+        <v>38.391756337771298</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B144" s="53">
+        <v>39.179463797191325</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B145" s="53">
+        <v>33.46270289987234</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B146" s="53">
+        <v>42.605690315520711</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B147" s="53">
+        <v>32.084442823271928</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B148" s="53">
+        <v>31.83695057450301</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B149" s="53">
+        <v>39.589959875980298</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B150" s="53">
+        <v>41.790990333758891</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" s="53">
+        <v>42.885828925770561</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B152" s="53">
+        <v>35.613167973737006</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B153" s="53">
+        <v>33.107058179828556</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B154" s="53">
+        <v>41.301842057267919</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B155" s="53">
+        <v>39.265912821448111</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B156" s="53">
+        <v>32.328469815794271</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B157" s="53">
+        <v>37.659675360204268</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B158" s="53">
+        <v>44.667335400328305</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B159" s="53">
+        <v>31.963341236549336</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B160" s="53">
+        <v>30.708371329564109</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B161" s="53">
+        <v>33.616268466168151</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B162" s="53">
+        <v>34.391026810140438</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B163" s="53">
+        <v>32.971366040488796</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B164" s="53">
+        <v>28.657851541127116</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B165" s="53">
+        <v>29.531096115265367</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B166" s="53">
+        <v>46.031369688126937</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B167" s="53">
+        <v>38.752507751231072</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B168" s="53">
+        <v>38.857377348167063</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B169" s="53">
+        <v>36.863395951121653</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B170" s="53">
+        <v>32.577603501732632</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B171" s="53">
+        <v>34.042631770928324</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B172" s="53">
+        <v>34.198978661316808</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B173" s="53">
+        <v>38.435345613715121</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B174" s="53">
+        <v>36.130585445923771</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B175" s="53">
+        <v>35.23227638675386</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B176" s="53">
+        <v>29.490789713660408</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B177" s="53">
+        <v>30.998358562830568</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B178" s="53">
+        <v>35.093118991167508</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B179" s="53">
+        <v>32.98084989968995</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B180" s="53">
+        <v>30.920116724420943</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B181" s="53">
+        <v>33.623381360569034</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.88671875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="31" t="s">
         <v>201</v>
       </c>
@@ -9157,7 +10632,7 @@
       <c r="N2" s="26"/>
       <c r="O2" s="26"/>
     </row>
-    <row r="3" spans="2:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="28"/>
       <c r="C3" s="24"/>
       <c r="D3" s="25"/>
@@ -9173,13 +10648,13 @@
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
     </row>
-    <row r="4" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29" t="s">
         <v>189</v>
       </c>
       <c r="C4" s="23"/>
     </row>
-    <row r="5" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>184</v>
       </c>
@@ -9187,7 +10662,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
         <v>185</v>
       </c>
@@ -9195,7 +10670,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>191</v>
       </c>
@@ -9203,22 +10678,22 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="21"/>
       <c r="C8" s="22" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="50" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="50" t="s">
         <v>186</v>
       </c>

</xml_diff>